<commit_message>
small update for times
</commit_message>
<xml_diff>
--- a/TurnInSchool/WorkingTimes.xlsx
+++ b/TurnInSchool/WorkingTimes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Week 1</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Verwacht weken</t>
+  </si>
+  <si>
+    <t>Uren</t>
   </si>
 </sst>
 </file>
@@ -640,14 +643,15 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,7 +717,9 @@
       <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,10 +949,13 @@
       <c r="B28" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
         <v>38</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>640</v>
       </c>
     </row>
@@ -955,12 +964,12 @@
         <v>33</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>39</v>
       </c>
-      <c r="E29">
-        <f>SUM(B2:F26)</f>
-        <v>8</v>
+      <c r="F29">
+        <f>SUM(C2:G26)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,12 +979,15 @@
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30">
+        <v>8.5</v>
+      </c>
+      <c r="E30" t="s">
         <v>37</v>
       </c>
-      <c r="E30">
-        <f>E29*8.5</f>
-        <v>68</v>
+      <c r="F30">
+        <f>F29*C30</f>
+        <v>76.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -983,30 +995,30 @@
         <v>35</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="E31">
-        <f>E28-E30</f>
-        <v>572</v>
+      <c r="F31">
+        <f>F28-F30</f>
+        <v>563.5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>41</v>
       </c>
-      <c r="E32">
-        <f>E31/8.5</f>
-        <v>67.294117647058826</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+      <c r="F32">
+        <f>F31/C30</f>
+        <v>66.294117647058826</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>42</v>
       </c>
-      <c r="E33">
-        <f>E32/4</f>
-        <v>16.823529411764707</v>
+      <c r="F33">
+        <f>F32/4</f>
+        <v>16.573529411764707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
times update with calculator hours
</commit_message>
<xml_diff>
--- a/TurnInSchool/WorkingTimes.xlsx
+++ b/TurnInSchool/WorkingTimes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Week 1</t>
   </si>
@@ -151,12 +151,24 @@
   </si>
   <si>
     <t>Uren</t>
+  </si>
+  <si>
+    <t>Days Calculator (H)</t>
+  </si>
+  <si>
+    <t>One day (H)</t>
+  </si>
+  <si>
+    <t>Answer: (Day)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -324,6 +336,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -640,18 +653,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,7 +746,7 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -746,7 +756,7 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -756,7 +766,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -766,7 +776,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -776,7 +786,7 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -786,7 +796,7 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -796,7 +806,7 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -806,7 +816,7 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -816,7 +826,7 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -826,7 +836,7 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -836,7 +846,7 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -846,7 +856,7 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -856,7 +866,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -866,7 +876,7 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
@@ -876,7 +886,7 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -886,7 +896,7 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -896,7 +906,7 @@
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -906,7 +916,7 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="12"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -916,7 +926,7 @@
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -926,7 +936,7 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -936,7 +946,7 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -955,7 +965,7 @@
       <c r="E28" t="s">
         <v>38</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="14">
         <v>640</v>
       </c>
     </row>
@@ -967,7 +977,7 @@
       <c r="E29" t="s">
         <v>39</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="14">
         <f>SUM(C2:G26)</f>
         <v>9</v>
       </c>
@@ -985,7 +995,7 @@
       <c r="E30" t="s">
         <v>37</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="14">
         <f>F29*C30</f>
         <v>76.5</v>
       </c>
@@ -998,7 +1008,7 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="14">
         <f>F28-F30</f>
         <v>563.5</v>
       </c>
@@ -1007,18 +1017,42 @@
       <c r="E32" t="s">
         <v>41</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="14">
         <f>F31/C30</f>
         <v>66.294117647058826</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
       <c r="E33" t="s">
         <v>42</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="14">
         <f>F32/4</f>
         <v>16.573529411764707</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <f>C30</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <f>B33/B34</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A update of all! Bad Commit name
</commit_message>
<xml_diff>
--- a/TurnInSchool/WorkingTimes.xlsx
+++ b/TurnInSchool/WorkingTimes.xlsx
@@ -656,7 +656,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +742,9 @@
       <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
@@ -983,7 +985,7 @@
       </c>
       <c r="F29" s="14">
         <f>SUM(C2:G26)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1003,7 @@
       </c>
       <c r="F30" s="14">
         <f>F29*C30</f>
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,7 +1016,7 @@
       </c>
       <c r="F31" s="14">
         <f>F28-F30</f>
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,7 +1025,7 @@
       </c>
       <c r="F32" s="14">
         <f>F31/C30</f>
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,7 +1040,7 @@
       </c>
       <c r="F33" s="14">
         <f>F32/4</f>
-        <v>17.25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>